<commit_message>
check in Advance Poll Voting Record
check in Advance Poll Voting Record
</commit_message>
<xml_diff>
--- a/campaign/Lawn Sign.Britannia.xlsx
+++ b/campaign/Lawn Sign.Britannia.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Britannia Woods" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Britannia Woods'!$A$1:$H$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Britannia Woods'!$A$1:$H$44</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="70">
   <si>
     <t>Street Number</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>TRAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Apache Court.</t>
+  </si>
+  <si>
+    <t>Chen</t>
   </si>
 </sst>
 </file>
@@ -656,10 +662,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H43"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -696,7 +703,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" s="6"/>
       <c r="B2" s="3">
         <v>533</v>
@@ -714,7 +721,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="6"/>
       <c r="B3" s="3">
         <v>552</v>
@@ -732,7 +739,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="6"/>
       <c r="B4" s="3">
         <v>531</v>
@@ -750,7 +757,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" s="6">
         <v>41153</v>
       </c>
@@ -770,7 +777,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="6">
         <v>41153</v>
       </c>
@@ -790,7 +797,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="6">
         <v>41153</v>
       </c>
@@ -810,7 +817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="6">
         <v>41153</v>
       </c>
@@ -830,7 +837,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="6">
         <v>41153</v>
       </c>
@@ -850,7 +857,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="6">
         <v>41153</v>
       </c>
@@ -870,7 +877,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" s="6">
         <v>41153</v>
       </c>
@@ -893,7 +900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" s="6">
         <v>41153</v>
       </c>
@@ -947,7 +954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="6">
         <v>41153</v>
       </c>
@@ -967,7 +974,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="6">
         <v>41153</v>
       </c>
@@ -987,7 +994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" hidden="1">
       <c r="A17" s="6">
         <v>43344</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" hidden="1">
       <c r="A18" s="6">
         <v>41153</v>
       </c>
@@ -1027,7 +1034,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" hidden="1">
       <c r="A19" s="6">
         <v>41153</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" hidden="1">
       <c r="A20" s="6">
         <v>43344</v>
       </c>
@@ -1065,7 +1072,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21" s="6">
         <v>41153</v>
       </c>
@@ -1079,8 +1086,11 @@
       <c r="E21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="H21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1">
       <c r="B22" s="2">
         <v>5186</v>
       </c>
@@ -1097,7 +1107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" hidden="1">
       <c r="A23" s="6">
         <v>41153</v>
       </c>
@@ -1117,7 +1127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" hidden="1">
       <c r="A24" s="6">
         <v>41153</v>
       </c>
@@ -1137,7 +1147,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" hidden="1">
       <c r="A25" s="6">
         <v>41153</v>
       </c>
@@ -1157,7 +1167,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" hidden="1">
       <c r="A26" s="6">
         <v>43344</v>
       </c>
@@ -1177,7 +1187,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" hidden="1">
       <c r="A27" s="6">
         <v>41153</v>
       </c>
@@ -1197,7 +1207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" hidden="1">
       <c r="A28" s="6"/>
       <c r="B28" s="3">
         <v>539</v>
@@ -1257,7 +1267,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" hidden="1">
       <c r="B32" s="2">
         <v>5519</v>
       </c>
@@ -1268,6 +1278,9 @@
         <v>49</v>
       </c>
       <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1281,6 +1294,9 @@
       <c r="D33" t="s">
         <v>51</v>
       </c>
+      <c r="F33" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="2">
@@ -1306,6 +1322,9 @@
       <c r="D35" t="s">
         <v>53</v>
       </c>
+      <c r="F35" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="2">
@@ -1321,7 +1340,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" hidden="1">
       <c r="B37" s="2">
         <v>5152</v>
       </c>
@@ -1338,7 +1357,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" hidden="1">
       <c r="B38" s="2">
         <v>539</v>
       </c>
@@ -1422,10 +1441,26 @@
         <v>31</v>
       </c>
     </row>
+    <row r="44" spans="2:8">
+      <c r="B44">
+        <v>460</v>
+      </c>
+      <c r="C44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F44" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H39">
+  <autoFilter ref="A1:H44">
     <filterColumn colId="4"/>
-    <filterColumn colId="7"/>
+    <filterColumn colId="7">
+      <filters blank="1"/>
+    </filterColumn>
   </autoFilter>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
check in lawn sign locations
check in lawn sign locations
</commit_message>
<xml_diff>
--- a/campaign/Lawn Sign.Britannia.xlsx
+++ b/campaign/Lawn Sign.Britannia.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
   <si>
     <t>Street Number</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>Chen</t>
+  </si>
+  <si>
+    <t>RIFFAT</t>
   </si>
 </sst>
 </file>
@@ -666,7 +669,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="B41" sqref="B41:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1409,6 +1412,9 @@
       <c r="C41" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="D41" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="E41" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
checking in AP08 file and small lawn sign
checking in AP08 file and small lawn sign
</commit_message>
<xml_diff>
--- a/campaign/Lawn Sign.Britannia.xlsx
+++ b/campaign/Lawn Sign.Britannia.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
   <si>
     <t>Street Number</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>RIFFAT</t>
+  </si>
+  <si>
+    <t>Guildwood Way</t>
+  </si>
+  <si>
+    <t>Starwood Dr</t>
   </si>
 </sst>
 </file>
@@ -666,10 +672,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:D42"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1461,6 +1467,121 @@
         <v>31</v>
       </c>
     </row>
+    <row r="45" spans="2:8">
+      <c r="B45">
+        <v>5256</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46">
+        <v>5076</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47">
+        <v>5088</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48">
+        <v>5104</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49">
+        <v>5160</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50">
+        <v>5194</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51">
+        <v>5240</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52">
+        <v>5036</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53">
+        <v>5096</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54">
+        <v>5447</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55">
+        <v>720</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H44">
     <filterColumn colId="4"/>

</xml_diff>

<commit_message>
committing lawn sign change and update the TrusteeEP_05
committing lawn sign change and update the TrusteeEP_05
</commit_message>
<xml_diff>
--- a/campaign/Lawn Sign.Britannia.xlsx
+++ b/campaign/Lawn Sign.Britannia.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="73">
   <si>
     <t>Street Number</t>
   </si>
@@ -672,10 +672,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1477,6 +1477,9 @@
       <c r="F45" t="s">
         <v>31</v>
       </c>
+      <c r="G45" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="46" spans="2:8">
       <c r="B46">
@@ -1488,6 +1491,9 @@
       <c r="F46" t="s">
         <v>31</v>
       </c>
+      <c r="G46" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="47" spans="2:8">
       <c r="B47">
@@ -1499,6 +1505,9 @@
       <c r="F47" t="s">
         <v>31</v>
       </c>
+      <c r="G47" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="48" spans="2:8">
       <c r="B48">
@@ -1510,8 +1519,11 @@
       <c r="F48" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="49" spans="2:6">
+      <c r="G48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7">
       <c r="B49">
         <v>5160</v>
       </c>
@@ -1521,8 +1533,11 @@
       <c r="F49" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="2:6">
+      <c r="G49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7">
       <c r="B50">
         <v>5194</v>
       </c>
@@ -1532,8 +1547,11 @@
       <c r="F50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="51" spans="2:6">
+      <c r="G50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7">
       <c r="B51">
         <v>5240</v>
       </c>
@@ -1543,8 +1561,11 @@
       <c r="F51" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="52" spans="2:6">
+      <c r="G51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7">
       <c r="B52">
         <v>5036</v>
       </c>
@@ -1554,8 +1575,11 @@
       <c r="F52" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="53" spans="2:6">
+      <c r="G52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7">
       <c r="B53">
         <v>5096</v>
       </c>
@@ -1565,8 +1589,11 @@
       <c r="F53" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="54" spans="2:6">
+      <c r="G53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7">
       <c r="B54">
         <v>5447</v>
       </c>
@@ -1574,12 +1601,56 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:7">
       <c r="B55">
         <v>720</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56">
+        <v>5145</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7">
+      <c r="B57">
+        <v>5065</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58">
+        <v>932</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7">
+      <c r="B59">
+        <v>720</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>